<commit_message>
Update for latest docs
- Add configuration_url
- Add entity_category
</commit_message>
<xml_diff>
--- a/Types.xlsx
+++ b/Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Git\Personal\MBW.HassMQTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0693F6-F4D5-4078-B29F-1A37B3873951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFAAAC5-41D8-4DD3-A3B3-3DEAC5AA4769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EAE53F03-9736-4DE6-A991-28625A0786A2}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EAE53F03-9736-4DE6-A991-28625A0786A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="48">
   <si>
     <t>Alarm control panels</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>retain</t>
+  </si>
+  <si>
+    <t>entity_category</t>
   </si>
 </sst>
 </file>
@@ -255,18 +258,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}" name="Table1" displayName="Table1" ref="A1:J19" totalsRowShown="0">
-  <autoFilter ref="A1:J19" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}">
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J19">
-    <sortCondition ref="A1:A19"/>
-  </sortState>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}" name="Table1" displayName="Table1" ref="A1:K19" totalsRowShown="0">
+  <autoFilter ref="A1:K19" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{94D88D1A-5069-4A2E-98F5-0B5766970493}" name="Type"/>
     <tableColumn id="2" xr3:uid="{0B3FB65F-E1FC-45ED-897A-E5A2860A9482}" name="Link" dataCellStyle="Hyperlink"/>
     <tableColumn id="9" xr3:uid="{46515115-72A5-4044-A8C4-1CCB05097181}" name="unique_id" dataCellStyle="Normal"/>
@@ -276,8 +270,9 @@
     <tableColumn id="4" xr3:uid="{7AE65AA2-1DBF-453C-B955-73FA9594956B}" name="icon"/>
     <tableColumn id="5" xr3:uid="{2F98B26C-AA6D-4A08-B05C-3951B278CEA0}" name="enabled_by_default"/>
     <tableColumn id="11" xr3:uid="{698F8231-EE89-4502-9A65-44F846390A6C}" name="retain"/>
+    <tableColumn id="8" xr3:uid="{79989F16-41E3-4D7B-AA6F-98A1790DEE88}" name="entity_category"/>
     <tableColumn id="10" xr3:uid="{AE46ED81-9DA4-429D-87A1-39A6482AB057}" name="C#" dataDxfId="0">
-      <calculatedColumnFormula>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</calculatedColumnFormula>
+      <calculatedColumnFormula>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -581,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962644DB-EB69-4AF7-8959-CB9EAAD2C662}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,11 +592,11 @@
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" customWidth="1"/>
+    <col min="9" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -630,10 +625,13 @@
         <v>46</v>
       </c>
       <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -661,12 +659,15 @@
       <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -691,12 +692,15 @@
       <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -718,12 +722,15 @@
       <c r="H4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -751,12 +758,15 @@
       <c r="I5" t="s">
         <v>38</v>
       </c>
-      <c r="J5" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -784,12 +794,15 @@
       <c r="I6" t="s">
         <v>38</v>
       </c>
-      <c r="J6" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -811,12 +824,12 @@
       <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="J7" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
+      <c r="K7" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
         <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -826,12 +839,12 @@
       <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="J8" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
+      <c r="K8" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
         <v>: MqttSensorDiscoveryBase, IHasQos</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -859,12 +872,15 @@
       <c r="I9" t="s">
         <v>38</v>
       </c>
-      <c r="J9" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -892,12 +908,15 @@
       <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="J10" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -925,12 +944,15 @@
       <c r="I11" t="s">
         <v>38</v>
       </c>
-      <c r="J11" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -958,12 +980,15 @@
       <c r="I12" t="s">
         <v>38</v>
       </c>
-      <c r="J12" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -991,12 +1016,15 @@
       <c r="I13" t="s">
         <v>38</v>
       </c>
-      <c r="J13" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1021,12 +1049,15 @@
       <c r="I14" t="s">
         <v>38</v>
       </c>
-      <c r="J14" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1054,12 +1085,15 @@
       <c r="I15" t="s">
         <v>38</v>
       </c>
-      <c r="J15" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1084,12 +1118,15 @@
       <c r="H16" t="s">
         <v>38</v>
       </c>
-      <c r="J16" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1117,24 +1154,27 @@
       <c r="I17" t="s">
         <v>38</v>
       </c>
-      <c r="J17" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J18" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
+      <c r="K18" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
         <v>: MqttSensorDiscoveryBase</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1162,13 +1202,16 @@
       <c r="I19" t="s">
         <v>38</v>
       </c>
-      <c r="J19" t="str">
-        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasRetain","")</f>
-        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain</v>
+      <c r="J19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")</f>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:I1048576">
+  <conditionalFormatting sqref="C1:J1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update for latest docs, add Siren
</commit_message>
<xml_diff>
--- a/Types.xlsx
+++ b/Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Git\Personal\MBW.HassMQTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45934AFE-8D35-4517-80B1-25D1FE8BAED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D47D982-76A4-477A-8104-8A0F04D9129A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EAE53F03-9736-4DE6-A991-28625A0786A2}"/>
+    <workbookView xWindow="5205" yWindow="1515" windowWidth="26850" windowHeight="17235" xr2:uid="{EAE53F03-9736-4DE6-A991-28625A0786A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="54">
   <si>
     <t>Alarm control panels</t>
   </si>
@@ -190,13 +190,19 @@
   </si>
   <si>
     <t>encoding</t>
+  </si>
+  <si>
+    <t>Siren</t>
+  </si>
+  <si>
+    <t>https://www.home-assistant.io/integrations/siren.mqtt/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,13 +218,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,17 +248,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -272,10 +293,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}" name="Table1" displayName="Table1" ref="A1:M20" totalsRowShown="0">
-  <autoFilter ref="A1:M20" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M20">
-    <sortCondition ref="A1:A20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}" name="Table1" displayName="Table1" ref="A1:M21" totalsRowShown="0">
+  <autoFilter ref="A1:M21" xr:uid="{8698B62C-5989-42CD-A364-E269CC9C72CC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M21">
+    <sortCondition ref="A1:A21"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94D88D1A-5069-4A2E-98F5-0B5766970493}" name="Type"/>
@@ -595,13 +616,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962644DB-EB69-4AF7-8959-CB9EAAD2C662}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,96 +1267,138 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J18" t="s">
-        <v>38</v>
-      </c>
-      <c r="K18" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M18" t="str">
+        <v>53</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="3" t="str">
         <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")&amp;IF(Table1[[#This Row],[object_id]]="x",", IHasObjectId","")&amp;IF(Table1[[#This Row],[encoding]]="x",", IHasEncoding","")</f>
         <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory, IHasObjectId, IHasEncoding</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" t="s">
+        <v>38</v>
       </c>
       <c r="M19" t="str">
         <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")&amp;IF(Table1[[#This Row],[object_id]]="x",", IHasObjectId","")&amp;IF(Table1[[#This Row],[encoding]]="x",", IHasEncoding","")</f>
-        <v>: MqttSensorDiscoveryBase</v>
+        <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory, IHasObjectId, IHasEncoding</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" t="str">
+        <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")&amp;IF(Table1[[#This Row],[object_id]]="x",", IHasObjectId","")&amp;IF(Table1[[#This Row],[encoding]]="x",", IHasEncoding","")</f>
+        <v>: MqttSensorDiscoveryBase</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" t="s">
-        <v>38</v>
-      </c>
-      <c r="L20" t="s">
-        <v>38</v>
-      </c>
-      <c r="M20" t="str">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" t="str">
         <f>": MqttSensorDiscoveryBase"&amp;IF(Table1[[#This Row],[unique_id]]="x",", IHasUniqueId","")&amp;IF(Table1[[#This Row],[availability]]="x",", IHasAvailability","")&amp;IF(Table1[[#This Row],[qos]]="x",", IHasQos","")&amp;IF(Table1[[#This Row],[json_attributes]]="x",", IHasJsonAttributes","")&amp;IF(Table1[[#This Row],[icon]]="x",", IHasIcon","")&amp;IF(Table1[[#This Row],[enabled_by_default]]="x",", IHasEnabledByDefault","")&amp;IF(Table1[[#This Row],[retain]]="x",", IHasRetain","")&amp;IF(Table1[[#This Row],[entity_category]]="x",", IHasEntityCategory","")&amp;IF(Table1[[#This Row],[object_id]]="x",", IHasObjectId","")&amp;IF(Table1[[#This Row],[encoding]]="x",", IHasEncoding","")</f>
         <v>: MqttSensorDiscoveryBase, IHasUniqueId, IHasAvailability, IHasQos, IHasJsonAttributes, IHasIcon, IHasEnabledByDefault, IHasRetain, IHasEntityCategory, IHasObjectId, IHasEncoding</v>
       </c>
@@ -1360,17 +1423,18 @@
     <hyperlink ref="B15" r:id="rId11" xr:uid="{E3A2337D-E888-4EA1-BC93-6FA89EA7E72D}"/>
     <hyperlink ref="B16" r:id="rId12" xr:uid="{2C2C5088-975F-4EE9-8DB7-FC88322963A2}"/>
     <hyperlink ref="B17" r:id="rId13" xr:uid="{7A14182C-E62F-4CC6-A390-8B1C397F1EDE}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{B5A40D1A-BBBD-48A6-9737-7786C7DEDC19}"/>
-    <hyperlink ref="B19" r:id="rId15" xr:uid="{6C287BC1-833E-48AC-8E4A-69358B9A374C}"/>
-    <hyperlink ref="B20" r:id="rId16" xr:uid="{43A22CED-4681-4F4E-86F1-ECA0AA884871}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{B5A40D1A-BBBD-48A6-9737-7786C7DEDC19}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{6C287BC1-833E-48AC-8E4A-69358B9A374C}"/>
+    <hyperlink ref="B21" r:id="rId16" xr:uid="{43A22CED-4681-4F4E-86F1-ECA0AA884871}"/>
     <hyperlink ref="B11" r:id="rId17" xr:uid="{E4BFF757-489A-494E-8E1A-ED96DDE3DC97}"/>
     <hyperlink ref="B12" r:id="rId18" xr:uid="{25781BC7-A1FF-4B47-8E98-59A7C0D8E2DD}"/>
     <hyperlink ref="B4" r:id="rId19" xr:uid="{3DEBD040-2913-46C5-952E-90D88CA01CF4}"/>
+    <hyperlink ref="B18" r:id="rId20" xr:uid="{F91157ED-71B3-423C-A671-11999B021A3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>